<commit_message>
regresja - poprawiona prezentacja
</commit_message>
<xml_diff>
--- a/data/german_credit_data.xlsx
+++ b/data/german_credit_data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\analiza-danych-R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4BE0B43-AED5-44CE-AB8A-922D4EF6BF7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93486237-DF2A-4A55-96AF-F3C4175D9725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="german_credit_data" sheetId="1" r:id="rId1"/>
+    <sheet name="new_customers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5433" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5614" uniqueCount="29">
   <si>
     <t>Age</t>
   </si>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -964,11 +965,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31282,4 +31283,1108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2034656F-0F43-4E2A-8FEA-386CC3282F08}">
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>3069</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>1740</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2353</v>
+      </c>
+      <c r="H4">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>3556</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>2397</v>
+      </c>
+      <c r="H6">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>454</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>1715</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>2520</v>
+      </c>
+      <c r="H9">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>3568</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>7166</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>3939</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>1514</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>7393</v>
+      </c>
+      <c r="H14">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>1193</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>7297</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>2831</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18">
+        <v>1258</v>
+      </c>
+      <c r="H18">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>753</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>2427</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>2538</v>
+      </c>
+      <c r="H21">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>1264</v>
+      </c>
+      <c r="H22">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23">
+        <v>8386</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>4844</v>
+      </c>
+      <c r="H24">
+        <v>48</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>2923</v>
+      </c>
+      <c r="H25">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26">
+        <v>8229</v>
+      </c>
+      <c r="H26">
+        <v>36</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27">
+        <v>2028</v>
+      </c>
+      <c r="H27">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28">
+        <v>1433</v>
+      </c>
+      <c r="H28">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>6289</v>
+      </c>
+      <c r="H29">
+        <v>42</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <v>1409</v>
+      </c>
+      <c r="H30">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31">
+        <v>6579</v>
+      </c>
+      <c r="H31">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <v>1743</v>
+      </c>
+      <c r="H32">
+        <v>24</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <v>3565</v>
+      </c>
+      <c r="H33">
+        <v>12</v>
+      </c>
+      <c r="I33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34">
+        <v>1569</v>
+      </c>
+      <c r="H34">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>1936</v>
+      </c>
+      <c r="H35">
+        <v>18</v>
+      </c>
+      <c r="I35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>3959</v>
+      </c>
+      <c r="H36">
+        <v>36</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>2390</v>
+      </c>
+      <c r="H37">
+        <v>12</v>
+      </c>
+      <c r="I37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38">
+        <v>1736</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39">
+        <v>3857</v>
+      </c>
+      <c r="H39">
+        <v>30</v>
+      </c>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40">
+        <v>804</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>